<commit_message>
Menambahkan ipynb dan mengupdate sprint project
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 7\ML\Praktikum\Modul 1\Tugas_Praktikum_1\TugPrak_ML-D_188-230\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736118D9-8A32-4EE7-A7EF-8A6E1F77CE94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2820149E-F4B9-4634-8AED-3AE99301BC91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{014A5D45-3AD2-46BF-BFC6-9D5E8AAA7414}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>No.</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>DataBase Desain</t>
-  </si>
-  <si>
     <t>PreProcessing</t>
   </si>
   <si>
@@ -79,13 +76,19 @@
   </si>
   <si>
     <t>Waiting</t>
+  </si>
+  <si>
+    <t>Pencarian dan Analisis Dataset</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +96,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +124,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -397,27 +426,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,9 +441,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -451,14 +464,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,14 +812,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224A46A4-2613-464D-B600-59EE640C73DE}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
@@ -790,162 +827,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="13"/>
+      <c r="D1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="17">
+      <c r="B4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="11">
         <v>44483</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="11">
         <v>44493</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>16</v>
+      <c r="E4" s="25">
+        <v>44491</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="14">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8">
         <v>44494</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="8">
         <v>44504</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>17</v>
+      <c r="E5" s="26">
+        <v>44493</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="14">
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8">
         <v>44505</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="8">
         <v>44515</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
+      <c r="E6" s="26">
+        <v>44495</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="B7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8">
         <v>44516</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="8">
         <v>44526</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>17</v>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="14">
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8">
         <v>44527</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="8">
         <v>44537</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>17</v>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="15">
+      <c r="B9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
         <v>44538</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="9">
         <v>44548</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>17</v>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>